<commit_message>
code format for printing, added abstract
</commit_message>
<xml_diff>
--- a/Workbook4.xlsx
+++ b/Workbook4.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
   <si>
-    <t>entries</t>
-  </si>
-  <si>
     <t>ways</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>Total Space Used</t>
+  </si>
+  <si>
+    <t>Sets</t>
   </si>
 </sst>
 </file>
@@ -180,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -250,18 +250,8 @@
       <name val="Times New Roman"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
       <i/>
       <sz val="12"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
     <font>
@@ -272,7 +262,34 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
@@ -291,27 +308,9 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="12">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="1">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal style="thin">
-        <color auto="1"/>
-      </diagonal>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -322,9 +321,7 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -342,50 +339,8 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -491,7 +446,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -567,104 +522,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -672,111 +563,145 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -814,6 +739,8 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -851,6 +778,8 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1182,529 +1111,504 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:S96"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4:S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="10" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="12">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="9">
         <v>1</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="9">
         <v>2</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <v>3</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="9">
         <v>4</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="9">
         <v>5</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="9">
         <v>6</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="9">
         <v>7</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="9">
         <v>8</v>
       </c>
       <c r="K3" s="7">
         <v>1</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
+      <c r="L3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="13">
+      <c r="A4" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="10">
         <v>8</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="23">
         <f>I33</f>
         <v>61</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="23">
         <f>I41</f>
         <v>123</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="23">
         <f>I49</f>
         <v>186</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="23">
         <f>I57</f>
         <v>249</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="23">
         <f>I65</f>
         <v>312</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="23">
         <f>I73</f>
         <v>376</v>
       </c>
-      <c r="I4" s="15">
+      <c r="I4" s="23">
         <f>I81</f>
         <v>440</v>
       </c>
-      <c r="J4" s="16">
+      <c r="J4" s="23">
         <f>I89</f>
         <v>504</v>
       </c>
       <c r="K4" s="7">
         <v>2</v>
       </c>
-      <c r="L4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
+      <c r="L4" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="37"/>
-      <c r="B5" s="13">
+      <c r="A5" s="22"/>
+      <c r="B5" s="10">
         <v>16</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="23">
         <f t="shared" ref="C5:C11" si="0">I34</f>
         <v>120</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="23">
         <f t="shared" ref="D5:D11" si="1">I42</f>
         <v>242</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="23">
         <f t="shared" ref="E5:E11" si="2">I50</f>
         <v>366</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="23">
         <f t="shared" ref="F5:F11" si="3">I58</f>
         <v>490</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="23">
         <f t="shared" ref="G5:G11" si="4">I66</f>
         <v>614</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="23">
         <f t="shared" ref="H5:H11" si="5">I74</f>
         <v>740</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="23">
         <f t="shared" ref="I5:I11" si="6">I82</f>
         <v>866</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="23">
         <f t="shared" ref="J5:J11" si="7">I90</f>
         <v>992</v>
       </c>
       <c r="K5" s="7">
         <v>3</v>
       </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="8"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="37"/>
-      <c r="B6" s="19">
-        <v>32</v>
-      </c>
-      <c r="C6" s="17">
+      <c r="A6" s="22"/>
+      <c r="B6" s="11">
+        <v>32</v>
+      </c>
+      <c r="C6" s="23">
         <f t="shared" si="0"/>
         <v>236</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="23">
         <f t="shared" si="1"/>
         <v>476</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="23">
         <f t="shared" si="2"/>
         <v>720</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="23">
         <f t="shared" si="3"/>
         <v>964</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="23">
         <f t="shared" si="4"/>
         <v>1208</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="23">
         <f t="shared" si="5"/>
         <v>1456</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="23">
         <f t="shared" si="6"/>
         <v>1704</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="23">
         <f t="shared" si="7"/>
         <v>1952</v>
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="37"/>
-      <c r="B7" s="19">
+      <c r="A7" s="22"/>
+      <c r="B7" s="11">
         <v>64</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="24">
         <f t="shared" si="0"/>
         <v>464</v>
       </c>
-      <c r="D7" s="39">
+      <c r="D7" s="24">
         <f t="shared" si="1"/>
         <v>936</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="24">
         <f t="shared" si="2"/>
         <v>1416</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="24">
         <f t="shared" si="3"/>
         <v>1896</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="25">
         <f t="shared" si="4"/>
         <v>2376</v>
       </c>
-      <c r="H7" s="43">
+      <c r="H7" s="25">
         <f t="shared" si="5"/>
         <v>2864</v>
       </c>
-      <c r="I7" s="43">
+      <c r="I7" s="25">
         <f t="shared" si="6"/>
         <v>3352</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="25">
         <f t="shared" si="7"/>
         <v>3840</v>
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="37"/>
-      <c r="B8" s="19">
+      <c r="A8" s="22"/>
+      <c r="B8" s="11">
         <v>128</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="24">
         <f t="shared" si="0"/>
         <v>912</v>
       </c>
-      <c r="D8" s="39">
+      <c r="D8" s="24">
         <f t="shared" si="1"/>
         <v>1840</v>
       </c>
-      <c r="E8" s="43">
+      <c r="E8" s="25">
         <f t="shared" si="2"/>
         <v>2784</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="25">
         <f t="shared" si="3"/>
         <v>3728</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="26">
         <f t="shared" si="4"/>
         <v>4672</v>
       </c>
-      <c r="H8" s="40">
+      <c r="H8" s="26">
         <f t="shared" si="5"/>
         <v>5632</v>
       </c>
-      <c r="I8" s="40">
+      <c r="I8" s="26">
         <f t="shared" si="6"/>
         <v>6592</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="26">
         <f t="shared" si="7"/>
         <v>7552</v>
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="37"/>
-      <c r="B9" s="19">
+      <c r="A9" s="22"/>
+      <c r="B9" s="11">
         <v>256</v>
       </c>
-      <c r="C9" s="38">
+      <c r="C9" s="24">
         <f t="shared" si="0"/>
         <v>1792</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="25">
         <f t="shared" si="1"/>
         <v>3616</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="26">
         <f t="shared" si="2"/>
         <v>5472</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="26">
         <f t="shared" si="3"/>
         <v>7328</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="26">
         <f t="shared" si="4"/>
         <v>9184</v>
       </c>
-      <c r="H9" s="40">
+      <c r="H9" s="26">
         <f t="shared" si="5"/>
         <v>11072</v>
       </c>
-      <c r="I9" s="40">
+      <c r="I9" s="26">
         <f t="shared" si="6"/>
         <v>12960</v>
       </c>
-      <c r="J9" s="41">
+      <c r="J9" s="26">
         <f t="shared" si="7"/>
         <v>14848</v>
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="37"/>
-      <c r="B10" s="19">
+      <c r="A10" s="22"/>
+      <c r="B10" s="11">
         <v>512</v>
       </c>
-      <c r="C10" s="44">
+      <c r="C10" s="25">
         <f t="shared" si="0"/>
         <v>3520</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="26">
         <f t="shared" si="1"/>
         <v>7104</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="26">
         <f t="shared" si="2"/>
         <v>10752</v>
       </c>
-      <c r="F10" s="40">
+      <c r="F10" s="26">
         <f t="shared" si="3"/>
         <v>14400</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="26">
         <f t="shared" si="4"/>
         <v>18048</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10" s="26">
         <f t="shared" si="5"/>
         <v>21760</v>
       </c>
-      <c r="I10" s="40">
+      <c r="I10" s="26">
         <f t="shared" si="6"/>
         <v>25472</v>
       </c>
-      <c r="J10" s="41">
+      <c r="J10" s="26">
         <f t="shared" si="7"/>
         <v>29184</v>
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="37"/>
-      <c r="B11" s="19">
+      <c r="A11" s="22"/>
+      <c r="B11" s="11">
         <v>1024</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="32">
         <f t="shared" si="0"/>
         <v>6912</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="32">
         <f t="shared" si="1"/>
         <v>13952</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="32">
         <f t="shared" si="2"/>
         <v>21120</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="32">
         <f t="shared" si="3"/>
         <v>28288</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="32">
         <f t="shared" si="4"/>
         <v>35456</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="32">
         <f t="shared" si="5"/>
         <v>42752</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="32">
         <f t="shared" si="6"/>
         <v>50048</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="32">
         <f t="shared" si="7"/>
         <v>57344</v>
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+    </row>
+    <row r="15" spans="1:19" ht="15" customHeight="1">
+      <c r="A15" s="22"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="C14" s="11">
-        <f>CEILING(LOG(FACT(C15),2),1)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="11">
-        <f>CEILING(LOG(FACT(D15),2),1)</f>
-        <v>1</v>
-      </c>
-      <c r="E14" s="11">
-        <f>CEILING(LOG(FACT(E15),2),1)</f>
+      <c r="D15" s="9">
+        <v>2</v>
+      </c>
+      <c r="E15" s="9">
         <v>3</v>
       </c>
-      <c r="F14" s="11">
-        <f t="shared" ref="F14:J14" si="8">CEILING(LOG(FACT(F15),2),1)</f>
+      <c r="F15" s="9">
+        <v>4</v>
+      </c>
+      <c r="G15" s="9">
         <v>5</v>
       </c>
-      <c r="G14" s="11">
+      <c r="H15" s="9">
+        <v>6</v>
+      </c>
+      <c r="I15" s="9">
+        <v>7</v>
+      </c>
+      <c r="J15" s="9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="22"/>
+      <c r="B16" s="11">
+        <v>32</v>
+      </c>
+      <c r="C16" s="33">
+        <f t="shared" ref="C16:H16" si="8">AVERAGE(L16:L19)</f>
+        <v>34.323880000000003</v>
+      </c>
+      <c r="D16" s="33">
         <f t="shared" si="8"/>
-        <v>7</v>
-      </c>
-      <c r="H14" s="11">
+        <v>28.460542499999999</v>
+      </c>
+      <c r="E16" s="33">
         <f t="shared" si="8"/>
-        <v>10</v>
-      </c>
-      <c r="I14" s="11">
+        <v>24.320625</v>
+      </c>
+      <c r="F16" s="33">
         <f t="shared" si="8"/>
-        <v>13</v>
-      </c>
-      <c r="J14" s="11">
+        <v>21.190035000000002</v>
+      </c>
+      <c r="G16" s="33">
         <f t="shared" si="8"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1">
-      <c r="A15" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="12">
-        <v>1</v>
-      </c>
-      <c r="D15" s="12">
-        <v>2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>3</v>
-      </c>
-      <c r="F15" s="12">
-        <v>4</v>
-      </c>
-      <c r="G15" s="12">
-        <v>5</v>
-      </c>
-      <c r="H15" s="12">
-        <v>6</v>
-      </c>
-      <c r="I15" s="12">
-        <v>7</v>
-      </c>
-      <c r="J15" s="12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="11">
-        <f>LOG(B16,2)</f>
-        <v>5</v>
-      </c>
-      <c r="B16" s="19">
-        <v>32</v>
-      </c>
-      <c r="C16" s="23">
-        <f t="shared" ref="C16:H16" si="9">AVERAGE(L16:L19)</f>
-        <v>34.323880000000003</v>
-      </c>
-      <c r="D16" s="24">
-        <f t="shared" si="9"/>
-        <v>28.460542499999999</v>
-      </c>
-      <c r="E16" s="24">
-        <f t="shared" si="9"/>
-        <v>24.320625</v>
-      </c>
-      <c r="F16" s="24">
-        <f t="shared" si="9"/>
-        <v>21.190035000000002</v>
-      </c>
-      <c r="G16" s="24">
-        <f t="shared" si="9"/>
         <v>19.4595375</v>
       </c>
-      <c r="H16" s="24">
-        <f t="shared" si="9"/>
+      <c r="H16" s="33">
+        <f t="shared" si="8"/>
         <v>18.59666</v>
       </c>
-      <c r="I16" s="24">
+      <c r="I16" s="33">
         <f>AVERAGE(R16:R19)</f>
         <v>18.115069999999999</v>
       </c>
-      <c r="J16" s="25">
+      <c r="J16" s="33">
         <f>AVERAGE(S16:S19)</f>
         <v>17.784765</v>
       </c>
@@ -1734,42 +1638,39 @@
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="11">
-        <f t="shared" ref="A17:A20" si="10">LOG(B17,2)</f>
-        <v>6</v>
-      </c>
-      <c r="B17" s="19">
+      <c r="A17" s="22"/>
+      <c r="B17" s="11">
         <v>64</v>
       </c>
-      <c r="C17" s="26">
-        <f t="shared" ref="C17:H17" si="11">AVERAGE(L20:L23)</f>
+      <c r="C17" s="27">
+        <f t="shared" ref="C17:H17" si="9">AVERAGE(L20:L23)</f>
         <v>29.483962500000001</v>
       </c>
       <c r="D17" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>21.793622500000001</v>
       </c>
       <c r="E17" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>19.285565000000002</v>
       </c>
       <c r="F17" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>18.029087499999999</v>
       </c>
       <c r="G17" s="27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>17.414845</v>
       </c>
       <c r="H17" s="28">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>17.083829999999999</v>
       </c>
       <c r="I17" s="28">
         <f>AVERAGE(R20:R23)</f>
         <v>16.873547500000001</v>
       </c>
-      <c r="J17" s="49">
+      <c r="J17" s="29">
         <f>AVERAGE(S20:S23)</f>
         <v>16.663134999999997</v>
       </c>
@@ -1799,38 +1700,35 @@
       </c>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="11">
+      <c r="A18" s="22"/>
+      <c r="B18" s="11">
+        <v>128</v>
+      </c>
+      <c r="C18" s="27">
+        <f t="shared" ref="C18:F18" si="10">AVERAGE(L24:L27)</f>
+        <v>25.173652500000003</v>
+      </c>
+      <c r="D18" s="27">
         <f t="shared" si="10"/>
-        <v>7</v>
-      </c>
-      <c r="B18" s="19">
-        <v>128</v>
-      </c>
-      <c r="C18" s="26">
-        <f t="shared" ref="C18:F18" si="12">AVERAGE(L24:L27)</f>
-        <v>25.173652500000003</v>
-      </c>
-      <c r="D18" s="27">
-        <f t="shared" si="12"/>
         <v>19.051275</v>
       </c>
       <c r="E18" s="28">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>17.604189999999999</v>
       </c>
-      <c r="F18" s="48">
-        <f t="shared" si="12"/>
+      <c r="F18" s="29">
+        <f t="shared" si="10"/>
         <v>16.748889999999999</v>
       </c>
       <c r="G18" s="27"/>
-      <c r="H18" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="29" t="s">
-        <v>2</v>
+      <c r="H18" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="30" t="s">
+        <v>1</v>
       </c>
       <c r="J18" s="30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L18" s="4">
         <v>17.920590000000001</v>
@@ -1858,14 +1756,11 @@
       </c>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="11">
-        <f t="shared" si="10"/>
-        <v>8</v>
-      </c>
-      <c r="B19" s="19">
+      <c r="A19" s="22"/>
+      <c r="B19" s="11">
         <v>256</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="33">
         <f>AVERAGE(L28:L31)</f>
         <v>20.7624675</v>
       </c>
@@ -1873,23 +1768,23 @@
         <f>AVERAGE(M28:M31)</f>
         <v>17.402304999999998</v>
       </c>
-      <c r="E19" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" s="29" t="s">
-        <v>2</v>
+      <c r="E19" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="30" t="s">
+        <v>1</v>
       </c>
       <c r="J19" s="30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L19" s="5">
         <v>57.773820000000001</v>
@@ -1917,37 +1812,34 @@
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="11">
-        <f t="shared" si="10"/>
-        <v>9</v>
-      </c>
-      <c r="B20" s="19">
+      <c r="A20" s="22"/>
+      <c r="B20" s="11">
         <v>512</v>
       </c>
-      <c r="C20" s="45">
+      <c r="C20" s="28">
         <f>AVERAGE(L32:L35)</f>
         <v>18.292355000000001</v>
       </c>
-      <c r="D20" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="G20" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20" s="47" t="s">
-        <v>2</v>
+      <c r="D20" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>1</v>
       </c>
       <c r="L20" s="3">
         <v>14.836169999999999</v>
@@ -1975,16 +1867,16 @@
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="11"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
+      <c r="A21" s="22"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
       <c r="L21" s="4">
         <v>33.34198</v>
       </c>
@@ -2011,16 +1903,16 @@
       </c>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
       <c r="L22" s="4">
         <v>14.312010000000001</v>
       </c>
@@ -2047,16 +1939,16 @@
       </c>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="50"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="50"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
       <c r="L23" s="5">
         <v>55.445689999999999</v>
       </c>
@@ -2083,16 +1975,16 @@
       </c>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
-      <c r="I24" s="51"/>
-      <c r="J24" s="51"/>
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
       <c r="L24" s="3">
         <v>9.8355300000000003</v>
       </c>
@@ -2110,16 +2002,16 @@
       </c>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="50"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
       <c r="L25" s="4">
         <v>25.59479</v>
       </c>
@@ -2137,16 +2029,16 @@
       </c>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="50"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
       <c r="L26" s="4">
         <v>12.4374</v>
       </c>
@@ -2164,16 +2056,16 @@
       </c>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" s="50"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
       <c r="L27" s="5">
         <v>52.826889999999999</v>
       </c>
@@ -2191,16 +2083,16 @@
       </c>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="50"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
-      <c r="H28" s="35"/>
-      <c r="I28" s="35"/>
-      <c r="J28" s="35"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
       <c r="L28" s="3">
         <v>7.2354599999999998</v>
       </c>
@@ -2209,16 +2101,16 @@
       </c>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="50"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-      <c r="J29" s="35"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
       <c r="L29" s="4">
         <v>14.325430000000001</v>
       </c>
@@ -2254,28 +2146,28 @@
     </row>
     <row r="32" spans="1:19">
       <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
         <v>38</v>
       </c>
-      <c r="C32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>39</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" t="s">
         <v>40</v>
       </c>
-      <c r="F32" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" t="s">
-        <v>25</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
         <v>41</v>
-      </c>
-      <c r="I32" t="s">
-        <v>42</v>
       </c>
       <c r="L32" s="3">
         <v>5.0268199999999998</v>
@@ -2323,26 +2215,26 @@
         <v>1</v>
       </c>
       <c r="D34">
-        <f t="shared" ref="D34:D96" si="13">CEILING(LOG(FACT(C34),2),1)</f>
+        <f t="shared" ref="D34:D96" si="11">CEILING(LOG(FACT(C34),2),1)</f>
         <v>0</v>
       </c>
       <c r="E34">
-        <f t="shared" ref="E34:E96" si="14">CEILING(LOG(B34,2),1)</f>
+        <f t="shared" ref="E34:E96" si="12">CEILING(LOG(B34,2),1)</f>
         <v>4</v>
       </c>
       <c r="F34">
         <v>32</v>
       </c>
       <c r="G34">
-        <f t="shared" ref="G34:G96" si="15">F34-E34</f>
+        <f t="shared" ref="G34:G96" si="13">F34-E34</f>
         <v>28</v>
       </c>
       <c r="H34">
-        <f t="shared" ref="H34:H96" si="16">B34*(D34+C34*(F34+G34))</f>
+        <f t="shared" ref="H34:H96" si="14">B34*(D34+C34*(F34+G34))</f>
         <v>960</v>
       </c>
       <c r="I34">
-        <f t="shared" ref="I34:I96" si="17">H34/8</f>
+        <f t="shared" ref="I34:I96" si="15">H34/8</f>
         <v>120</v>
       </c>
       <c r="L34" s="4">
@@ -2357,26 +2249,26 @@
         <v>1</v>
       </c>
       <c r="D35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E35">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="F35">
         <v>32</v>
       </c>
       <c r="G35">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="H35">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>1888</v>
       </c>
       <c r="I35">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>236</v>
       </c>
       <c r="L35" s="5">
@@ -2391,26 +2283,26 @@
         <v>1</v>
       </c>
       <c r="D36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E36">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="F36">
         <v>32</v>
       </c>
       <c r="G36">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="H36">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>3712</v>
       </c>
       <c r="I36">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>464</v>
       </c>
     </row>
@@ -2422,26 +2314,26 @@
         <v>1</v>
       </c>
       <c r="D37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E37">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="F37">
         <v>32</v>
       </c>
       <c r="G37">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="H37">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>7296</v>
       </c>
       <c r="I37">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>912</v>
       </c>
     </row>
@@ -2453,26 +2345,26 @@
         <v>1</v>
       </c>
       <c r="D38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="F38">
         <v>32</v>
       </c>
       <c r="G38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="H38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>14336</v>
       </c>
       <c r="I38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1792</v>
       </c>
     </row>
@@ -2484,26 +2376,26 @@
         <v>1</v>
       </c>
       <c r="D39">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="F39">
         <v>32</v>
       </c>
       <c r="G39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="H39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>28160</v>
       </c>
       <c r="I39">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>3520</v>
       </c>
     </row>
@@ -2515,26 +2407,26 @@
         <v>1</v>
       </c>
       <c r="D40">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="E40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="F40">
         <v>32</v>
       </c>
       <c r="G40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="H40">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>55296</v>
       </c>
       <c r="I40">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>6912</v>
       </c>
     </row>
@@ -2546,26 +2438,26 @@
         <v>2</v>
       </c>
       <c r="D41">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E41">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="F41">
         <v>32</v>
       </c>
       <c r="G41">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="H41">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>984</v>
       </c>
       <c r="I41">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>123</v>
       </c>
     </row>
@@ -2577,26 +2469,26 @@
         <v>2</v>
       </c>
       <c r="D42">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E42">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="F42">
         <v>32</v>
       </c>
       <c r="G42">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="H42">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>1936</v>
       </c>
       <c r="I42">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>242</v>
       </c>
     </row>
@@ -2608,26 +2500,26 @@
         <v>2</v>
       </c>
       <c r="D43">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E43">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="F43">
         <v>32</v>
       </c>
       <c r="G43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="H43">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>3808</v>
       </c>
       <c r="I43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>476</v>
       </c>
     </row>
@@ -2639,26 +2531,26 @@
         <v>2</v>
       </c>
       <c r="D44">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E44">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="F44">
         <v>32</v>
       </c>
       <c r="G44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="H44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>7488</v>
       </c>
       <c r="I44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>936</v>
       </c>
     </row>
@@ -2670,26 +2562,26 @@
         <v>2</v>
       </c>
       <c r="D45">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E45">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="F45">
         <v>32</v>
       </c>
       <c r="G45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="H45">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>14720</v>
       </c>
       <c r="I45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1840</v>
       </c>
     </row>
@@ -2701,26 +2593,26 @@
         <v>2</v>
       </c>
       <c r="D46">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E46">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="F46">
         <v>32</v>
       </c>
       <c r="G46">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="H46">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>28928</v>
       </c>
       <c r="I46">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>3616</v>
       </c>
     </row>
@@ -2732,26 +2624,26 @@
         <v>2</v>
       </c>
       <c r="D47">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E47">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="F47">
         <v>32</v>
       </c>
       <c r="G47">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="H47">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>56832</v>
       </c>
       <c r="I47">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>7104</v>
       </c>
     </row>
@@ -2763,26 +2655,26 @@
         <v>2</v>
       </c>
       <c r="D48">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="E48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="F48">
         <v>32</v>
       </c>
       <c r="G48">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="H48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>111616</v>
       </c>
       <c r="I48">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>13952</v>
       </c>
     </row>
@@ -2794,26 +2686,26 @@
         <v>3</v>
       </c>
       <c r="D49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E49">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="F49">
         <v>32</v>
       </c>
       <c r="G49">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="H49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>1488</v>
       </c>
       <c r="I49">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>186</v>
       </c>
     </row>
@@ -2825,26 +2717,26 @@
         <v>3</v>
       </c>
       <c r="D50">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E50">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="F50">
         <v>32</v>
       </c>
       <c r="G50">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="H50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>2928</v>
       </c>
       <c r="I50">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>366</v>
       </c>
     </row>
@@ -2856,26 +2748,26 @@
         <v>3</v>
       </c>
       <c r="D51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E51">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="F51">
         <v>32</v>
       </c>
       <c r="G51">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="H51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>5760</v>
       </c>
       <c r="I51">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>720</v>
       </c>
     </row>
@@ -2887,26 +2779,26 @@
         <v>3</v>
       </c>
       <c r="D52">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E52">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="F52">
         <v>32</v>
       </c>
       <c r="G52">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="H52">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>11328</v>
       </c>
       <c r="I52">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1416</v>
       </c>
     </row>
@@ -2918,26 +2810,26 @@
         <v>3</v>
       </c>
       <c r="D53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E53">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="F53">
         <v>32</v>
       </c>
       <c r="G53">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="H53">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>22272</v>
       </c>
       <c r="I53">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>2784</v>
       </c>
     </row>
@@ -2949,26 +2841,26 @@
         <v>3</v>
       </c>
       <c r="D54">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E54">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="F54">
         <v>32</v>
       </c>
       <c r="G54">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="H54">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>43776</v>
       </c>
       <c r="I54">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>5472</v>
       </c>
     </row>
@@ -2980,26 +2872,26 @@
         <v>3</v>
       </c>
       <c r="D55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E55">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="F55">
         <v>32</v>
       </c>
       <c r="G55">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="H55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>86016</v>
       </c>
       <c r="I55">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>10752</v>
       </c>
     </row>
@@ -3011,26 +2903,26 @@
         <v>3</v>
       </c>
       <c r="D56">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="E56">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="F56">
         <v>32</v>
       </c>
       <c r="G56">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="H56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>168960</v>
       </c>
       <c r="I56">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>21120</v>
       </c>
     </row>
@@ -3042,26 +2934,26 @@
         <v>4</v>
       </c>
       <c r="D57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="E57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="F57">
         <v>32</v>
       </c>
       <c r="G57">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="H57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>1992</v>
       </c>
       <c r="I57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>249</v>
       </c>
     </row>
@@ -3073,26 +2965,26 @@
         <v>4</v>
       </c>
       <c r="D58">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="E58">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="F58">
         <v>32</v>
       </c>
       <c r="G58">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="H58">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>3920</v>
       </c>
       <c r="I58">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>490</v>
       </c>
     </row>
@@ -3104,26 +2996,26 @@
         <v>4</v>
       </c>
       <c r="D59">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="E59">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="F59">
         <v>32</v>
       </c>
       <c r="G59">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="H59">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>7712</v>
       </c>
       <c r="I59">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>964</v>
       </c>
     </row>
@@ -3135,26 +3027,26 @@
         <v>4</v>
       </c>
       <c r="D60">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="E60">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="F60">
         <v>32</v>
       </c>
       <c r="G60">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="H60">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>15168</v>
       </c>
       <c r="I60">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1896</v>
       </c>
     </row>
@@ -3166,26 +3058,26 @@
         <v>4</v>
       </c>
       <c r="D61">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="E61">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="F61">
         <v>32</v>
       </c>
       <c r="G61">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="H61">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>29824</v>
       </c>
       <c r="I61">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>3728</v>
       </c>
     </row>
@@ -3197,26 +3089,26 @@
         <v>4</v>
       </c>
       <c r="D62">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="E62">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="F62">
         <v>32</v>
       </c>
       <c r="G62">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="H62">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>58624</v>
       </c>
       <c r="I62">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>7328</v>
       </c>
     </row>
@@ -3228,26 +3120,26 @@
         <v>4</v>
       </c>
       <c r="D63">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="E63">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="F63">
         <v>32</v>
       </c>
       <c r="G63">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="H63">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>115200</v>
       </c>
       <c r="I63">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>14400</v>
       </c>
     </row>
@@ -3259,26 +3151,26 @@
         <v>4</v>
       </c>
       <c r="D64">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="E64">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="F64">
         <v>32</v>
       </c>
       <c r="G64">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="H64">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>226304</v>
       </c>
       <c r="I64">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>28288</v>
       </c>
     </row>
@@ -3290,26 +3182,26 @@
         <v>5</v>
       </c>
       <c r="D65">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="E65">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="F65">
         <v>32</v>
       </c>
       <c r="G65">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="H65">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>2496</v>
       </c>
       <c r="I65">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>312</v>
       </c>
     </row>
@@ -3321,26 +3213,26 @@
         <v>5</v>
       </c>
       <c r="D66">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="E66">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="F66">
         <v>32</v>
       </c>
       <c r="G66">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="H66">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>4912</v>
       </c>
       <c r="I66">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>614</v>
       </c>
     </row>
@@ -3352,26 +3244,26 @@
         <v>5</v>
       </c>
       <c r="D67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="E67">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="F67">
         <v>32</v>
       </c>
       <c r="G67">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="H67">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>9664</v>
       </c>
       <c r="I67">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1208</v>
       </c>
     </row>
@@ -3383,26 +3275,26 @@
         <v>5</v>
       </c>
       <c r="D68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="E68">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="F68">
         <v>32</v>
       </c>
       <c r="G68">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="H68">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>19008</v>
       </c>
       <c r="I68">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>2376</v>
       </c>
     </row>
@@ -3414,26 +3306,26 @@
         <v>5</v>
       </c>
       <c r="D69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="E69">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="F69">
         <v>32</v>
       </c>
       <c r="G69">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="H69">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>37376</v>
       </c>
       <c r="I69">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>4672</v>
       </c>
     </row>
@@ -3445,26 +3337,26 @@
         <v>5</v>
       </c>
       <c r="D70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="E70">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="F70">
         <v>32</v>
       </c>
       <c r="G70">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="H70">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>73472</v>
       </c>
       <c r="I70">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>9184</v>
       </c>
     </row>
@@ -3476,26 +3368,26 @@
         <v>5</v>
       </c>
       <c r="D71">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="E71">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="F71">
         <v>32</v>
       </c>
       <c r="G71">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="H71">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>144384</v>
       </c>
       <c r="I71">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>18048</v>
       </c>
     </row>
@@ -3507,26 +3399,26 @@
         <v>5</v>
       </c>
       <c r="D72">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="E72">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="F72">
         <v>32</v>
       </c>
       <c r="G72">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="H72">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>283648</v>
       </c>
       <c r="I72">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>35456</v>
       </c>
     </row>
@@ -3538,26 +3430,26 @@
         <v>6</v>
       </c>
       <c r="D73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="E73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="F73">
         <v>32</v>
       </c>
       <c r="G73">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="H73">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>3008</v>
       </c>
       <c r="I73">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>376</v>
       </c>
     </row>
@@ -3569,26 +3461,26 @@
         <v>6</v>
       </c>
       <c r="D74">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="E74">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="F74">
         <v>32</v>
       </c>
       <c r="G74">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="H74">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>5920</v>
       </c>
       <c r="I74">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>740</v>
       </c>
     </row>
@@ -3600,26 +3492,26 @@
         <v>6</v>
       </c>
       <c r="D75">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="E75">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="F75">
         <v>32</v>
       </c>
       <c r="G75">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="H75">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>11648</v>
       </c>
       <c r="I75">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1456</v>
       </c>
     </row>
@@ -3631,26 +3523,26 @@
         <v>6</v>
       </c>
       <c r="D76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="E76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="F76">
         <v>32</v>
       </c>
       <c r="G76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="H76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>22912</v>
       </c>
       <c r="I76">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>2864</v>
       </c>
     </row>
@@ -3662,26 +3554,26 @@
         <v>6</v>
       </c>
       <c r="D77">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="E77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="F77">
         <v>32</v>
       </c>
       <c r="G77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="H77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>45056</v>
       </c>
       <c r="I77">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>5632</v>
       </c>
     </row>
@@ -3693,26 +3585,26 @@
         <v>6</v>
       </c>
       <c r="D78">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="E78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="F78">
         <v>32</v>
       </c>
       <c r="G78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="H78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>88576</v>
       </c>
       <c r="I78">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>11072</v>
       </c>
     </row>
@@ -3724,26 +3616,26 @@
         <v>6</v>
       </c>
       <c r="D79">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="E79">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="F79">
         <v>32</v>
       </c>
       <c r="G79">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="H79">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>174080</v>
       </c>
       <c r="I79">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>21760</v>
       </c>
     </row>
@@ -3755,26 +3647,26 @@
         <v>6</v>
       </c>
       <c r="D80">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="E80">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="F80">
         <v>32</v>
       </c>
       <c r="G80">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="H80">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>342016</v>
       </c>
       <c r="I80">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>42752</v>
       </c>
     </row>
@@ -3786,26 +3678,26 @@
         <v>7</v>
       </c>
       <c r="D81">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="E81">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="F81">
         <v>32</v>
       </c>
       <c r="G81">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="H81">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>3520</v>
       </c>
       <c r="I81">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>440</v>
       </c>
     </row>
@@ -3817,26 +3709,26 @@
         <v>7</v>
       </c>
       <c r="D82">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="E82">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="F82">
         <v>32</v>
       </c>
       <c r="G82">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="H82">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>6928</v>
       </c>
       <c r="I82">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>866</v>
       </c>
     </row>
@@ -3848,26 +3740,26 @@
         <v>7</v>
       </c>
       <c r="D83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="E83">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="F83">
         <v>32</v>
       </c>
       <c r="G83">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="H83">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>13632</v>
       </c>
       <c r="I83">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1704</v>
       </c>
     </row>
@@ -3879,26 +3771,26 @@
         <v>7</v>
       </c>
       <c r="D84">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="E84">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="F84">
         <v>32</v>
       </c>
       <c r="G84">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="H84">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>26816</v>
       </c>
       <c r="I84">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>3352</v>
       </c>
     </row>
@@ -3910,26 +3802,26 @@
         <v>7</v>
       </c>
       <c r="D85">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="E85">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="F85">
         <v>32</v>
       </c>
       <c r="G85">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="H85">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>52736</v>
       </c>
       <c r="I85">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>6592</v>
       </c>
     </row>
@@ -3941,26 +3833,26 @@
         <v>7</v>
       </c>
       <c r="D86">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="E86">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="F86">
         <v>32</v>
       </c>
       <c r="G86">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="H86">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>103680</v>
       </c>
       <c r="I86">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>12960</v>
       </c>
     </row>
@@ -3972,26 +3864,26 @@
         <v>7</v>
       </c>
       <c r="D87">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="E87">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="F87">
         <v>32</v>
       </c>
       <c r="G87">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="H87">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>203776</v>
       </c>
       <c r="I87">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>25472</v>
       </c>
     </row>
@@ -4003,26 +3895,26 @@
         <v>7</v>
       </c>
       <c r="D88">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
       <c r="E88">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="F88">
         <v>32</v>
       </c>
       <c r="G88">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="H88">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>400384</v>
       </c>
       <c r="I88">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>50048</v>
       </c>
     </row>
@@ -4034,26 +3926,26 @@
         <v>8</v>
       </c>
       <c r="D89">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="E89">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="F89">
         <v>32</v>
       </c>
       <c r="G89">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>29</v>
       </c>
       <c r="H89">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>4032</v>
       </c>
       <c r="I89">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>504</v>
       </c>
     </row>
@@ -4065,26 +3957,26 @@
         <v>8</v>
       </c>
       <c r="D90">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="E90">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="F90">
         <v>32</v>
       </c>
       <c r="G90">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>28</v>
       </c>
       <c r="H90">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>7936</v>
       </c>
       <c r="I90">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>992</v>
       </c>
     </row>
@@ -4096,26 +3988,26 @@
         <v>8</v>
       </c>
       <c r="D91">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="E91">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="F91">
         <v>32</v>
       </c>
       <c r="G91">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>27</v>
       </c>
       <c r="H91">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>15616</v>
       </c>
       <c r="I91">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>1952</v>
       </c>
     </row>
@@ -4127,26 +4019,26 @@
         <v>8</v>
       </c>
       <c r="D92">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="E92">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="F92">
         <v>32</v>
       </c>
       <c r="G92">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>26</v>
       </c>
       <c r="H92">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>30720</v>
       </c>
       <c r="I92">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>3840</v>
       </c>
     </row>
@@ -4158,26 +4050,26 @@
         <v>8</v>
       </c>
       <c r="D93">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="E93">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="F93">
         <v>32</v>
       </c>
       <c r="G93">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>25</v>
       </c>
       <c r="H93">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>60416</v>
       </c>
       <c r="I93">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>7552</v>
       </c>
     </row>
@@ -4189,26 +4081,26 @@
         <v>8</v>
       </c>
       <c r="D94">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="E94">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="F94">
         <v>32</v>
       </c>
       <c r="G94">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="H94">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>118784</v>
       </c>
       <c r="I94">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>14848</v>
       </c>
     </row>
@@ -4220,26 +4112,26 @@
         <v>8</v>
       </c>
       <c r="D95">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="E95">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="F95">
         <v>32</v>
       </c>
       <c r="G95">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="H95">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>233472</v>
       </c>
       <c r="I95">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>29184</v>
       </c>
     </row>
@@ -4251,31 +4143,33 @@
         <v>8</v>
       </c>
       <c r="D96">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>16</v>
       </c>
       <c r="E96">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>10</v>
       </c>
       <c r="F96">
         <v>32</v>
       </c>
       <c r="G96">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>22</v>
       </c>
       <c r="H96">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>458752</v>
       </c>
       <c r="I96">
-        <f t="shared" si="17"/>
+        <f t="shared" si="15"/>
         <v>57344</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A14:A21"/>
+    <mergeCell ref="C14:J14"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="L3:S3"/>
     <mergeCell ref="L4:S4"/>
@@ -4333,382 +4227,382 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" style="10" customWidth="1"/>
-    <col min="4" max="5" width="11" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="10"/>
+    <col min="1" max="1" width="12.83203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" style="8" customWidth="1"/>
+    <col min="4" max="5" width="11" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" ht="16" customHeight="1">
-      <c r="A3" s="53" t="s">
+    <row r="3" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A3" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A4" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="53" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="80" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="81" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="B4" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="55" t="s">
+      <c r="C4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="D4" s="40">
+        <v>10240</v>
+      </c>
+      <c r="E4" s="41">
+        <f t="shared" ref="E4:E12" si="0">D4/8</f>
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A5" s="42"/>
+      <c r="B5" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="82">
-        <v>10240</v>
-      </c>
-      <c r="E4" s="83">
-        <f>D4/8</f>
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="16" customHeight="1">
-      <c r="A5" s="56"/>
-      <c r="B5" s="55" t="s">
+      <c r="C5" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="55" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="82">
+      <c r="D5" s="40">
         <f>1024*3</f>
         <v>3072</v>
       </c>
-      <c r="E5" s="84">
-        <f>D5/8</f>
+      <c r="E5" s="43">
+        <f t="shared" si="0"/>
         <v>384</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="16" customHeight="1">
-      <c r="A6" s="56"/>
-      <c r="B6" s="55" t="s">
+    <row r="6" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A6" s="42"/>
+      <c r="B6" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="55" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="82">
+      <c r="D6" s="40">
         <f>4096*2</f>
         <v>8192</v>
       </c>
-      <c r="E6" s="84">
-        <f>D6/8</f>
+      <c r="E6" s="43">
+        <f t="shared" si="0"/>
         <v>1024</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="16" customHeight="1">
-      <c r="A7" s="56"/>
-      <c r="B7" s="55" t="s">
+    <row r="7" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A7" s="42"/>
+      <c r="B7" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="82">
+      <c r="D7" s="40">
         <f>4096*2</f>
         <v>8192</v>
       </c>
-      <c r="E7" s="84">
-        <f>D7/8</f>
+      <c r="E7" s="43">
+        <f t="shared" si="0"/>
         <v>1024</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="16" customHeight="1">
-      <c r="A8" s="57"/>
-      <c r="B8" s="55" t="s">
+    <row r="8" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A8" s="44"/>
+      <c r="B8" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="82">
+      <c r="D8" s="40">
         <v>12</v>
       </c>
-      <c r="E8" s="85">
-        <f>D8/8</f>
+      <c r="E8" s="45">
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="16" customHeight="1">
-      <c r="A9" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="76">
+    <row r="9" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A9" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="47"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="49">
         <f>SUM(D4:D8)</f>
         <v>29708</v>
       </c>
-      <c r="E9" s="77">
-        <f>D9/8</f>
+      <c r="E9" s="50">
+        <f t="shared" si="0"/>
         <v>3713.5</v>
       </c>
-      <c r="F9" s="61"/>
-    </row>
-    <row r="10" spans="1:6" ht="16" customHeight="1">
-      <c r="A10" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="55" t="s">
+      <c r="F9" s="51"/>
+    </row>
+    <row r="10" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A10" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="55" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="82">
+      <c r="D10" s="40">
         <f>16*64</f>
         <v>1024</v>
       </c>
-      <c r="E10" s="83">
-        <f>D10/8</f>
+      <c r="E10" s="41">
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16" customHeight="1">
-      <c r="A11" s="63"/>
-      <c r="B11" s="55" t="s">
+    <row r="11" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A11" s="53"/>
+      <c r="B11" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="82">
+      <c r="D11" s="40">
         <f>32*64*8</f>
         <v>16384</v>
       </c>
-      <c r="E11" s="84">
-        <f>D11/8</f>
+      <c r="E11" s="43">
+        <f t="shared" si="0"/>
         <v>2048</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" customHeight="1">
-      <c r="A12" s="64"/>
-      <c r="B12" s="55" t="s">
+    <row r="12" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A12" s="54"/>
+      <c r="B12" s="39" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="82">
+      <c r="D12" s="40">
         <f>26*64*8</f>
         <v>13312</v>
       </c>
-      <c r="E12" s="85">
-        <f>D12/8</f>
+      <c r="E12" s="45">
+        <f t="shared" si="0"/>
         <v>1664</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" customHeight="1">
-      <c r="A13" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="59"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="76">
+    <row r="13" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A13" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="47"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="49">
         <f>SUM(D10:D12)</f>
         <v>30720</v>
       </c>
-      <c r="E13" s="77">
+      <c r="E13" s="50">
         <f>SUM(E10:E12)</f>
         <v>3840</v>
       </c>
-      <c r="F13" s="61"/>
-    </row>
-    <row r="14" spans="1:6" ht="16" customHeight="1">
-      <c r="A14" s="65" t="s">
+      <c r="F13" s="51"/>
+    </row>
+    <row r="14" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A14" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="55" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="82">
+      <c r="C14" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="40">
         <f>33*32</f>
         <v>1056</v>
       </c>
-      <c r="E14" s="83">
+      <c r="E14" s="41">
         <f>D14/8</f>
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="16" customHeight="1">
-      <c r="A15" s="66"/>
-      <c r="B15" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="82">
+    <row r="15" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A15" s="56"/>
+      <c r="B15" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="40">
         <v>6</v>
       </c>
-      <c r="E15" s="84">
+      <c r="E15" s="43">
         <f>D15/8</f>
         <v>0.75</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="16" customHeight="1">
-      <c r="A16" s="67"/>
-      <c r="B16" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="55" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="82">
+    <row r="16" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A16" s="57"/>
+      <c r="B16" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="40">
         <v>6</v>
       </c>
-      <c r="E16" s="85">
+      <c r="E16" s="45">
         <f>D16/8</f>
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" customHeight="1">
-      <c r="A17" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="76">
+    <row r="17" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A17" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="47"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49">
         <f>SUM(D14:D16)</f>
         <v>1068</v>
       </c>
-      <c r="E17" s="77">
+      <c r="E17" s="50">
         <f>SUM(E14:E16)</f>
         <v>133.5</v>
       </c>
-      <c r="F17" s="61"/>
-    </row>
-    <row r="18" spans="1:6" ht="16" customHeight="1">
-      <c r="A18" s="54" t="s">
+      <c r="F17" s="51"/>
+    </row>
+    <row r="18" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A18" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="75" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="55" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="86">
+      <c r="D18" s="59">
         <f>16*8</f>
         <v>128</v>
       </c>
-      <c r="E18" s="86">
+      <c r="E18" s="59">
         <f>D18/8</f>
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16" customHeight="1">
-      <c r="A19" s="56"/>
-      <c r="B19" s="68" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="84">
+    <row r="19" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A19" s="42"/>
+      <c r="B19" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="43">
         <f>32*8*8</f>
         <v>2048</v>
       </c>
-      <c r="E19" s="84">
+      <c r="E19" s="43">
         <f>D19/8</f>
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="16" customHeight="1">
-      <c r="A20" s="56"/>
-      <c r="B20" s="68" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="85">
+    <row r="20" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A20" s="42"/>
+      <c r="B20" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="45">
         <f>29*8*8</f>
         <v>1856</v>
       </c>
-      <c r="E20" s="84">
+      <c r="E20" s="43">
         <f>D20/8</f>
         <v>232</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="16" customHeight="1">
-      <c r="A21" s="58" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="79">
+    <row r="21" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A21" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="47"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="61">
         <f>SUM(D18:D20)</f>
         <v>4032</v>
       </c>
-      <c r="E21" s="78">
+      <c r="E21" s="62">
         <f>D21/8</f>
         <v>504</v>
       </c>
-      <c r="F21" s="61"/>
-    </row>
-    <row r="22" spans="1:6" ht="16" customHeight="1">
-      <c r="A22" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="70"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="87">
+      <c r="F21" s="51"/>
+    </row>
+    <row r="22" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A22" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" s="64"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="66">
         <f>D9+D13+D17+D21</f>
         <v>65528</v>
       </c>
-      <c r="E22" s="87">
+      <c r="E22" s="66">
         <f>E9+E13+E17+E21</f>
         <v>8191</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" customHeight="1">
-      <c r="A23" s="72" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="73"/>
-      <c r="C23" s="74"/>
-      <c r="D23" s="80">
+    <row r="23" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A23" s="67" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="35">
         <f>E23*8</f>
         <v>65536</v>
       </c>
-      <c r="E23" s="88">
+      <c r="E23" s="70">
         <v>8192</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="16" customHeight="1">
-      <c r="A24" s="69" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="70"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="89">
+    <row r="24" spans="1:6" s="37" customFormat="1" ht="14" customHeight="1">
+      <c r="A24" s="63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="64"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="71">
         <f>D23-D22</f>
         <v>8</v>
       </c>
-      <c r="E24" s="87">
+      <c r="E24" s="66">
         <f>E23-E22</f>
         <v>1</v>
       </c>

</xml_diff>